<commit_message>
Update S2026 data, mappings, and player hub fixes
</commit_message>
<xml_diff>
--- a/Name_email_mapping.xlsx
+++ b/Name_email_mapping.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -196,16 +199,16 @@
     <t>Danny Ji</t>
   </si>
   <si>
+    <t>Dji</t>
+  </si>
+  <si>
+    <t>danjispam@gmail.com</t>
+  </si>
+  <si>
+    <t>Danny Li</t>
+  </si>
+  <si>
     <t>Dli</t>
-  </si>
-  <si>
-    <t>danjispam@gmail.com</t>
-  </si>
-  <si>
-    <t>Danny LI</t>
-  </si>
-  <si>
-    <t>Dji</t>
   </si>
   <si>
     <t>lidanny2024@gmail.com</t>
@@ -769,24 +772,28 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -794,50 +801,65 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="5">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -864,22 +886,82 @@
         <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -891,157 +973,186 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr fitToPage="1"/>
+    <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.88"/>
-    <col customWidth="1" min="3" max="3" width="24.88"/>
+    <col min="1" max="1" style="4" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1063,15 +1174,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1082,87 +1194,97 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1173,7 +1295,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
@@ -1184,15 +1306,16 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -1203,55 +1326,61 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="B20" s="3"/>
       <c r="C20" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="B21" s="3"/>
       <c r="C21" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
       <c r="A22" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
       <c r="A25" s="2" t="s">
         <v>54</v>
       </c>
@@ -1262,7 +1391,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
@@ -1273,7 +1402,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
       <c r="A27" s="2" t="s">
         <v>60</v>
       </c>
@@ -1284,7 +1413,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
       <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
@@ -1295,15 +1424,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="B29" s="3"/>
       <c r="C29" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
       <c r="A30" s="2" t="s">
         <v>68</v>
       </c>
@@ -1314,7 +1444,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
       <c r="A31" s="2" t="s">
         <v>71</v>
       </c>
@@ -1325,31 +1455,34 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
       <c r="A32" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="B32" s="3"/>
       <c r="C32" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
       <c r="A33" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="B33" s="3"/>
       <c r="C33" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="B34" s="3"/>
       <c r="C34" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="35">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
       <c r="A35" s="2" t="s">
         <v>80</v>
       </c>
@@ -1360,55 +1493,61 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
       <c r="A36" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="37">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="B37" s="3"/>
       <c r="C37" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
       <c r="A38" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="B38" s="3"/>
       <c r="C38" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
       <c r="A39" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="B39" s="3"/>
       <c r="C39" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="40">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
       <c r="A40" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="B40" s="3"/>
       <c r="C40" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
       <c r="A41" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="B41" s="3"/>
       <c r="C41" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
       <c r="A42" s="2" t="s">
         <v>95</v>
       </c>
@@ -1419,31 +1558,34 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
       <c r="A43" s="2" t="s">
         <v>98</v>
       </c>
+      <c r="B43" s="3"/>
       <c r="C43" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="44">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
       <c r="A44" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="B44" s="3"/>
       <c r="C44" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="45">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
       <c r="A45" s="2" t="s">
         <v>102</v>
       </c>
+      <c r="B45" s="3"/>
       <c r="C45" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
       <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
@@ -1454,7 +1596,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="47">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
       <c r="A47" s="2" t="s">
         <v>107</v>
       </c>
@@ -1465,79 +1607,88 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
       <c r="A48" s="2" t="s">
         <v>110</v>
       </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="49">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
       <c r="A49" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
       <c r="A50" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="51">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
       <c r="A51" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="B51" s="3"/>
       <c r="C51" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="52">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
       <c r="A52" s="2" t="s">
         <v>118</v>
       </c>
+      <c r="B52" s="3"/>
       <c r="C52" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
       <c r="A53" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="B53" s="3"/>
       <c r="C53" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="54">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
       <c r="A54" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="B54" s="3"/>
       <c r="C54" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="55">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
       <c r="A55" s="2" t="s">
         <v>124</v>
       </c>
+      <c r="B55" s="3"/>
       <c r="C55" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="56">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
       <c r="A56" s="2" t="s">
         <v>126</v>
       </c>
+      <c r="B56" s="3"/>
       <c r="C56" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
       <c r="A57" s="2" t="s">
         <v>128</v>
       </c>
@@ -1548,7 +1699,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
       <c r="A58" s="2" t="s">
         <v>131</v>
       </c>
@@ -1559,23 +1710,25 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
       <c r="A59" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="B59" s="3"/>
       <c r="C59" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="60">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
       <c r="A60" s="2" t="s">
         <v>136</v>
       </c>
+      <c r="B60" s="3"/>
       <c r="C60" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="61">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
       <c r="A61" s="2" t="s">
         <v>138</v>
       </c>
@@ -1586,31 +1739,34 @@
         <v>140</v>
       </c>
     </row>
-    <row r="62">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
       <c r="A62" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="B62" s="3"/>
       <c r="C62" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="63">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
       <c r="A63" s="2" t="s">
         <v>143</v>
       </c>
+      <c r="B63" s="3"/>
       <c r="C63" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="64">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
       <c r="A64" s="2" t="s">
         <v>145</v>
       </c>
+      <c r="B64" s="3"/>
       <c r="C64" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="65">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
       <c r="A65" s="2" t="s">
         <v>147</v>
       </c>
@@ -1621,23 +1777,25 @@
         <v>149</v>
       </c>
     </row>
-    <row r="66">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
       <c r="A66" s="2" t="s">
         <v>150</v>
       </c>
+      <c r="B66" s="3"/>
       <c r="C66" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="67">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
       <c r="A67" s="2" t="s">
         <v>152</v>
       </c>
+      <c r="B67" s="3"/>
       <c r="C67" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="68">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
       <c r="A68" s="2" t="s">
         <v>154</v>
       </c>
@@ -1648,7 +1806,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="69">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
       <c r="A69" s="2" t="s">
         <v>157</v>
       </c>
@@ -1659,7 +1817,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25">
       <c r="A70" s="2" t="s">
         <v>160</v>
       </c>
@@ -1670,7 +1828,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
       <c r="A71" s="2" t="s">
         <v>163</v>
       </c>
@@ -1681,7 +1839,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="72">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25">
       <c r="A72" s="2" t="s">
         <v>166</v>
       </c>
@@ -1692,39 +1850,43 @@
         <v>168</v>
       </c>
     </row>
-    <row r="73">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25">
       <c r="A73" s="2" t="s">
         <v>169</v>
       </c>
+      <c r="B73" s="3"/>
       <c r="C73" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="74">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25">
       <c r="A74" s="2" t="s">
         <v>171</v>
       </c>
+      <c r="B74" s="3"/>
       <c r="C74" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="75">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
       <c r="A75" s="2" t="s">
         <v>173</v>
       </c>
+      <c r="B75" s="3"/>
       <c r="C75" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="76">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25">
       <c r="A76" s="2" t="s">
         <v>175</v>
       </c>
+      <c r="B76" s="3"/>
       <c r="C76" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="77">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
       <c r="A77" s="2" t="s">
         <v>177</v>
       </c>
@@ -1735,39 +1897,43 @@
         <v>179</v>
       </c>
     </row>
-    <row r="78">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
       <c r="A78" s="2" t="s">
         <v>180</v>
       </c>
+      <c r="B78" s="3"/>
       <c r="C78" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="79">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25">
       <c r="A79" s="2" t="s">
         <v>182</v>
       </c>
+      <c r="B79" s="3"/>
       <c r="C79" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="80">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
       <c r="A80" s="2" t="s">
         <v>184</v>
       </c>
+      <c r="B80" s="3"/>
       <c r="C80" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="81">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25">
       <c r="A81" s="2" t="s">
         <v>186</v>
       </c>
+      <c r="B81" s="3"/>
       <c r="C81" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="82">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25">
       <c r="A82" s="2" t="s">
         <v>188</v>
       </c>
@@ -1778,31 +1944,34 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25">
       <c r="A83" s="2" t="s">
         <v>191</v>
       </c>
+      <c r="B83" s="3"/>
       <c r="C83" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="84">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25">
       <c r="A84" s="2" t="s">
         <v>193</v>
       </c>
+      <c r="B84" s="3"/>
       <c r="C84" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="85">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25">
       <c r="A85" s="2" t="s">
         <v>195</v>
       </c>
+      <c r="B85" s="3"/>
       <c r="C85" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="86">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25">
       <c r="A86" s="2" t="s">
         <v>197</v>
       </c>
@@ -1813,63 +1982,70 @@
         <v>199</v>
       </c>
     </row>
-    <row r="87">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25">
       <c r="A87" s="2" t="s">
         <v>200</v>
       </c>
+      <c r="B87" s="3"/>
       <c r="C87" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="88">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25">
       <c r="A88" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="B88" s="3"/>
       <c r="C88" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="89">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
       <c r="A89" s="2" t="s">
         <v>204</v>
       </c>
+      <c r="B89" s="3"/>
       <c r="C89" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="90">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25">
       <c r="A90" s="2" t="s">
         <v>206</v>
       </c>
+      <c r="B90" s="3"/>
       <c r="C90" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="91">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25">
       <c r="A91" s="2" t="s">
         <v>208</v>
       </c>
+      <c r="B91" s="3"/>
       <c r="C91" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="92">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18">
       <c r="A92" s="2" t="s">
         <v>210</v>
       </c>
+      <c r="B92" s="3"/>
       <c r="C92" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="93">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18">
       <c r="A93" s="2" t="s">
         <v>212</v>
       </c>
+      <c r="B93" s="3"/>
       <c r="C93" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="94">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18">
       <c r="A94" s="2" t="s">
         <v>214</v>
       </c>
@@ -1880,7 +2056,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="95">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18">
       <c r="A95" s="2" t="s">
         <v>217</v>
       </c>
@@ -1891,7 +2067,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="96">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18">
       <c r="A96" s="2" t="s">
         <v>220</v>
       </c>
@@ -1902,23 +2078,25 @@
         <v>222</v>
       </c>
     </row>
-    <row r="97">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18">
       <c r="A97" s="2" t="s">
         <v>223</v>
       </c>
+      <c r="B97" s="3"/>
       <c r="C97" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="98">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25">
       <c r="A98" s="2" t="s">
         <v>225</v>
       </c>
+      <c r="B98" s="3"/>
       <c r="C98" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="99">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25">
       <c r="A99" s="2" t="s">
         <v>227</v>
       </c>
@@ -1929,23 +2107,25 @@
         <v>229</v>
       </c>
     </row>
-    <row r="100">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="17.25">
       <c r="A100" s="2" t="s">
         <v>230</v>
       </c>
+      <c r="B100" s="3"/>
       <c r="C100" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="101">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25">
       <c r="A101" s="2" t="s">
         <v>232</v>
       </c>
+      <c r="B101" s="3"/>
       <c r="C101" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="102">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="17.25">
       <c r="A102" s="2" t="s">
         <v>234</v>
       </c>
@@ -1956,66 +2136,70 @@
         <v>236</v>
       </c>
     </row>
-    <row r="103">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25">
       <c r="A103" s="2" t="s">
         <v>237</v>
       </c>
+      <c r="B103" s="3"/>
       <c r="C103" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="104">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25">
       <c r="A104" s="2" t="s">
         <v>239</v>
       </c>
+      <c r="B104" s="3"/>
       <c r="C104" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="105">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25">
       <c r="A105" s="2" t="s">
         <v>241</v>
       </c>
+      <c r="B105" s="3"/>
       <c r="C105" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="106">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25">
       <c r="A106" s="2" t="s">
         <v>243</v>
       </c>
+      <c r="B106" s="3"/>
       <c r="C106" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="107">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25">
       <c r="A107" s="2" t="s">
         <v>245</v>
       </c>
+      <c r="B107" s="3"/>
       <c r="C107" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="108">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25">
       <c r="A108" s="2" t="s">
         <v>247</v>
       </c>
+      <c r="B108" s="3"/>
       <c r="C108" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="109">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25">
       <c r="A109" s="2" t="s">
         <v>249</v>
       </c>
+      <c r="B109" s="3"/>
       <c r="C109" s="2" t="s">
         <v>250</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="1" horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>